<commit_message>
Update Index META DATA
</commit_message>
<xml_diff>
--- a/dataset_competition/META_DATA.xlsx
+++ b/dataset_competition/META_DATA.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hanbin Seo\bro.py\dataset_competition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seolab/bro.py/dataset_competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" tabRatio="681" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="26580" windowHeight="14900" tabRatio="681" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="테이블" sheetId="2" r:id="rId1"/>
@@ -29,9 +29,15 @@
     <definedName name="OTHER_IDX">변수설명_이외변수!$B$427</definedName>
     <definedName name="US_IDX">변수설명_이외변수!$B$95</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="1141">
   <si>
     <t>SPX</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -556,21 +562,21 @@
     <t>회사채 AA- 3년</t>
   </si>
   <si>
-    <t xml:space="preserve">YSR(국고채권(5년))_x000D_
+    <t xml:space="preserve">YSR(국고채권(5년))
 </t>
   </si>
   <si>
     <t>국고채5년 - CD</t>
   </si>
   <si>
-    <t xml:space="preserve">YSR(국고채권(10년))_x000D_
+    <t xml:space="preserve">YSR(국고채권(10년))
 </t>
   </si>
   <si>
     <t>국고채10년 - 통안채1년</t>
   </si>
   <si>
-    <t xml:space="preserve">YSR(3Y)_x000D_
+    <t xml:space="preserve">YSR(3Y)
 </t>
   </si>
   <si>
@@ -3568,18 +3574,66 @@
   </si>
   <si>
     <t>aGLFUCRY_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXUSDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXJPYD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXEURD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXJPDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXDERD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXDUKD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXDAUD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXCNDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXSWDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXHKDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXTHDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>arKOFXINDD_YoY</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -3905,16 +3959,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4027,10 +4081,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -4099,8 +4153,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4131,8 +4185,8 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4252,6 +4306,15 @@
     <cellStyle name="60% - Accent4" xfId="18"/>
     <cellStyle name="60% - Accent5" xfId="19"/>
     <cellStyle name="60% - Accent6" xfId="20"/>
+    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="백분율 2" xfId="53"/>
+    <cellStyle name="스타일 1" xfId="2"/>
+    <cellStyle name="콤마 [0]_일일금융시장_new" xfId="21"/>
+    <cellStyle name="콤마_일일금융시장_new" xfId="22"/>
+    <cellStyle name="표준 2" xfId="23"/>
+    <cellStyle name="표준 3" xfId="54"/>
+    <cellStyle name="표준 4" xfId="1"/>
+    <cellStyle name="하이퍼링크" xfId="55" builtinId="8"/>
     <cellStyle name="Accent1" xfId="24"/>
     <cellStyle name="Accent2" xfId="25"/>
     <cellStyle name="Accent3" xfId="26"/>
@@ -4281,15 +4344,6 @@
     <cellStyle name="Title" xfId="50"/>
     <cellStyle name="Total" xfId="51"/>
     <cellStyle name="Warning Text" xfId="52"/>
-    <cellStyle name="백분율 2" xfId="53"/>
-    <cellStyle name="스타일 1" xfId="2"/>
-    <cellStyle name="콤마 [0]_일일금융시장_new" xfId="21"/>
-    <cellStyle name="콤마_일일금융시장_new" xfId="22"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="23"/>
-    <cellStyle name="표준 3" xfId="54"/>
-    <cellStyle name="표준 4" xfId="1"/>
-    <cellStyle name="하이퍼링크" xfId="55" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4571,14 +4625,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="3" width="29.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -4595,7 +4649,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -4612,7 +4666,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -4629,7 +4683,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -4646,7 +4700,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -4663,7 +4717,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1063</v>
       </c>
@@ -4680,7 +4734,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1064</v>
       </c>
@@ -4697,7 +4751,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1065</v>
       </c>
@@ -4714,7 +4768,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>100</v>
       </c>
@@ -4731,7 +4785,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>495</v>
       </c>
@@ -4748,7 +4802,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>496</v>
       </c>
@@ -4765,7 +4819,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>494</v>
       </c>
@@ -4782,7 +4836,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>498</v>
       </c>
@@ -4799,7 +4853,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>497</v>
       </c>
@@ -4816,7 +4870,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>500</v>
       </c>
@@ -4833,7 +4887,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>499</v>
       </c>
@@ -4850,7 +4904,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>501</v>
       </c>
@@ -4892,13 +4946,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="29.125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>258</v>
       </c>
@@ -4906,7 +4960,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4914,7 +4968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4922,7 +4976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4930,7 +4984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4938,7 +4992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4946,7 +5000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4954,7 +5008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -4962,7 +5016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -4970,7 +5024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -4978,7 +5032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -4986,7 +5040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -5006,13 +5060,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="29.125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>258</v>
       </c>
@@ -5020,7 +5074,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -5028,7 +5082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5036,7 +5090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -5044,7 +5098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -5052,7 +5106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5060,7 +5114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5078,27 +5132,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="B313" sqref="B313:B392"/>
+    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="C440" sqref="C440"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="22.375" customWidth="1"/>
-    <col min="3" max="4" width="36.25" customWidth="1"/>
-    <col min="5" max="5" width="14.375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.25" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="4" width="36.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1071</v>
       </c>
@@ -5124,7 +5178,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5150,7 +5204,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5176,7 +5230,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5202,7 +5256,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5228,7 +5282,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5254,7 +5308,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5280,7 +5334,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5306,7 +5360,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5332,7 +5386,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5358,7 +5412,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5384,7 +5438,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5410,7 +5464,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5436,7 +5490,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5462,7 +5516,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5488,7 +5542,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5514,7 +5568,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5540,7 +5594,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5566,7 +5620,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5592,7 +5646,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5618,7 +5672,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -5644,7 +5698,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -5670,7 +5724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -5696,7 +5750,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -5722,7 +5776,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -5748,7 +5802,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -5774,7 +5828,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -5800,7 +5854,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -5826,7 +5880,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -5852,7 +5906,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -5878,7 +5932,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -5904,12 +5958,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>1070</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>1071</v>
       </c>
@@ -5935,7 +5989,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -5961,7 +6015,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -5987,7 +6041,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3</v>
       </c>
@@ -6013,7 +6067,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>4</v>
       </c>
@@ -6039,7 +6093,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>5</v>
       </c>
@@ -6065,7 +6119,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>6</v>
       </c>
@@ -6091,7 +6145,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>7</v>
       </c>
@@ -6117,7 +6171,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>8</v>
       </c>
@@ -6143,7 +6197,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>9</v>
       </c>
@@ -6169,7 +6223,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>10</v>
       </c>
@@ -6195,7 +6249,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>11</v>
       </c>
@@ -6221,7 +6275,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>12</v>
       </c>
@@ -6247,7 +6301,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>13</v>
       </c>
@@ -6273,7 +6327,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>14</v>
       </c>
@@ -6299,7 +6353,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>15</v>
       </c>
@@ -6325,7 +6379,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>16</v>
       </c>
@@ -6351,7 +6405,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>17</v>
       </c>
@@ -6377,7 +6431,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>18</v>
       </c>
@@ -6403,7 +6457,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>19</v>
       </c>
@@ -6429,7 +6483,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>20</v>
       </c>
@@ -6455,7 +6509,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>21</v>
       </c>
@@ -6481,7 +6535,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>22</v>
       </c>
@@ -6507,7 +6561,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>23</v>
       </c>
@@ -6533,7 +6587,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>24</v>
       </c>
@@ -6559,7 +6613,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>25</v>
       </c>
@@ -6585,7 +6639,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>26</v>
       </c>
@@ -6611,7 +6665,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>27</v>
       </c>
@@ -6637,7 +6691,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>28</v>
       </c>
@@ -6663,7 +6717,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>29</v>
       </c>
@@ -6689,7 +6743,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>30</v>
       </c>
@@ -6715,7 +6769,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>31</v>
       </c>
@@ -6741,7 +6795,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>32</v>
       </c>
@@ -6767,7 +6821,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>33</v>
       </c>
@@ -6793,7 +6847,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>34</v>
       </c>
@@ -6819,7 +6873,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>35</v>
       </c>
@@ -6845,7 +6899,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>36</v>
       </c>
@@ -6871,7 +6925,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>37</v>
       </c>
@@ -6897,7 +6951,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>38</v>
       </c>
@@ -6923,7 +6977,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>39</v>
       </c>
@@ -6949,7 +7003,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>40</v>
       </c>
@@ -6975,7 +7029,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>41</v>
       </c>
@@ -7001,7 +7055,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>42</v>
       </c>
@@ -7027,7 +7081,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43</v>
       </c>
@@ -7053,7 +7107,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44</v>
       </c>
@@ -7079,7 +7133,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45</v>
       </c>
@@ -7105,7 +7159,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>46</v>
       </c>
@@ -7131,7 +7185,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>47</v>
       </c>
@@ -7157,7 +7211,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>48</v>
       </c>
@@ -7183,7 +7237,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>49</v>
       </c>
@@ -7209,7 +7263,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>50</v>
       </c>
@@ -7235,7 +7289,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>51</v>
       </c>
@@ -7261,7 +7315,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>52</v>
       </c>
@@ -7287,7 +7341,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>53</v>
       </c>
@@ -7313,7 +7367,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>54</v>
       </c>
@@ -7339,7 +7393,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>55</v>
       </c>
@@ -7365,7 +7419,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>56</v>
       </c>
@@ -7391,7 +7445,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>57</v>
       </c>
@@ -7417,7 +7471,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>58</v>
       </c>
@@ -7443,12 +7497,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>1071</v>
       </c>
@@ -7474,7 +7528,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>1</v>
       </c>
@@ -7500,7 +7554,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2</v>
       </c>
@@ -7526,7 +7580,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>3</v>
       </c>
@@ -7552,7 +7606,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>4</v>
       </c>
@@ -7578,7 +7632,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>5</v>
       </c>
@@ -7604,7 +7658,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>6</v>
       </c>
@@ -7630,7 +7684,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="11">
         <v>7</v>
       </c>
@@ -7656,7 +7710,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>8</v>
       </c>
@@ -7682,7 +7736,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>9</v>
       </c>
@@ -7708,7 +7762,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>10</v>
       </c>
@@ -7734,7 +7788,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>11</v>
       </c>
@@ -7760,7 +7814,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>12</v>
       </c>
@@ -7786,7 +7840,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>13</v>
       </c>
@@ -7812,7 +7866,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>14</v>
       </c>
@@ -7838,7 +7892,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>15</v>
       </c>
@@ -7864,7 +7918,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>16</v>
       </c>
@@ -7890,7 +7944,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="10">
         <v>17</v>
       </c>
@@ -7916,7 +7970,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>18</v>
       </c>
@@ -7942,7 +7996,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>19</v>
       </c>
@@ -7968,7 +8022,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>20</v>
       </c>
@@ -7994,7 +8048,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>21</v>
       </c>
@@ -8020,7 +8074,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>22</v>
       </c>
@@ -8046,7 +8100,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>23</v>
       </c>
@@ -8072,7 +8126,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>24</v>
       </c>
@@ -8098,7 +8152,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>25</v>
       </c>
@@ -8124,7 +8178,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>26</v>
       </c>
@@ -8150,7 +8204,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>27</v>
       </c>
@@ -8176,7 +8230,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>28</v>
       </c>
@@ -8202,7 +8256,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>29</v>
       </c>
@@ -8228,7 +8282,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>30</v>
       </c>
@@ -8254,7 +8308,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>31</v>
       </c>
@@ -8280,7 +8334,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>32</v>
       </c>
@@ -8306,7 +8360,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>33</v>
       </c>
@@ -8332,7 +8386,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>34</v>
       </c>
@@ -8358,7 +8412,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>35</v>
       </c>
@@ -8384,7 +8438,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>36</v>
       </c>
@@ -8410,7 +8464,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>37</v>
       </c>
@@ -8436,7 +8490,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>38</v>
       </c>
@@ -8462,7 +8516,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="11">
         <v>39</v>
       </c>
@@ -8488,7 +8542,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="11">
         <v>40</v>
       </c>
@@ -8514,7 +8568,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>41</v>
       </c>
@@ -8540,7 +8594,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>42</v>
       </c>
@@ -8566,7 +8620,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>43</v>
       </c>
@@ -8592,7 +8646,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44</v>
       </c>
@@ -8618,7 +8672,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>45</v>
       </c>
@@ -8644,7 +8698,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>46</v>
       </c>
@@ -8670,7 +8724,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>47</v>
       </c>
@@ -8696,7 +8750,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>48</v>
       </c>
@@ -8722,7 +8776,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>49</v>
       </c>
@@ -8748,7 +8802,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>50</v>
       </c>
@@ -8774,7 +8828,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>51</v>
       </c>
@@ -8800,7 +8854,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>52</v>
       </c>
@@ -8826,7 +8880,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>53</v>
       </c>
@@ -8852,7 +8906,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>54</v>
       </c>
@@ -8878,7 +8932,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>55</v>
       </c>
@@ -8904,7 +8958,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>56</v>
       </c>
@@ -8930,7 +8984,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>57</v>
       </c>
@@ -8956,7 +9010,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>58</v>
       </c>
@@ -8982,7 +9036,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>59</v>
       </c>
@@ -9008,7 +9062,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>60</v>
       </c>
@@ -9034,7 +9088,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>61</v>
       </c>
@@ -9060,7 +9114,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>62</v>
       </c>
@@ -9086,7 +9140,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>63</v>
       </c>
@@ -9112,7 +9166,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="11">
         <v>64</v>
       </c>
@@ -9138,7 +9192,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>65</v>
       </c>
@@ -9164,7 +9218,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>66</v>
       </c>
@@ -9190,7 +9244,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="11">
         <v>67</v>
       </c>
@@ -9216,7 +9270,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>68</v>
       </c>
@@ -9242,7 +9296,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="11">
         <v>69</v>
       </c>
@@ -9268,7 +9322,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>70</v>
       </c>
@@ -9294,7 +9348,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>71</v>
       </c>
@@ -9320,7 +9374,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>72</v>
       </c>
@@ -9346,7 +9400,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>73</v>
       </c>
@@ -9372,7 +9426,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>74</v>
       </c>
@@ -9398,7 +9452,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>75</v>
       </c>
@@ -9422,7 +9476,7 @@
       </c>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>76</v>
       </c>
@@ -9446,7 +9500,7 @@
       </c>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>77</v>
       </c>
@@ -9472,7 +9526,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>78</v>
       </c>
@@ -9498,12 +9552,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B176" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>1071</v>
       </c>
@@ -9529,7 +9583,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>1</v>
       </c>
@@ -9555,7 +9609,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="11">
         <v>2</v>
       </c>
@@ -9581,7 +9635,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>3</v>
       </c>
@@ -9607,7 +9661,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>4</v>
       </c>
@@ -9633,7 +9687,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>5</v>
       </c>
@@ -9659,7 +9713,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>6</v>
       </c>
@@ -9685,7 +9739,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>7</v>
       </c>
@@ -9711,7 +9765,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>8</v>
       </c>
@@ -9737,7 +9791,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="11">
         <v>9</v>
       </c>
@@ -9763,7 +9817,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>10</v>
       </c>
@@ -9789,7 +9843,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>11</v>
       </c>
@@ -9815,7 +9869,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>12</v>
       </c>
@@ -9841,7 +9895,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>13</v>
       </c>
@@ -9867,7 +9921,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>14</v>
       </c>
@@ -9893,7 +9947,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>15</v>
       </c>
@@ -9919,7 +9973,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>16</v>
       </c>
@@ -9945,7 +9999,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>17</v>
       </c>
@@ -9971,7 +10025,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>18</v>
       </c>
@@ -9997,7 +10051,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="11">
         <v>19</v>
       </c>
@@ -10023,7 +10077,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>20</v>
       </c>
@@ -10049,7 +10103,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>21</v>
       </c>
@@ -10075,7 +10129,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>22</v>
       </c>
@@ -10101,7 +10155,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>23</v>
       </c>
@@ -10127,7 +10181,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>24</v>
       </c>
@@ -10153,7 +10207,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>25</v>
       </c>
@@ -10179,7 +10233,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>26</v>
       </c>
@@ -10205,7 +10259,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>27</v>
       </c>
@@ -10231,7 +10285,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>28</v>
       </c>
@@ -10257,7 +10311,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>29</v>
       </c>
@@ -10283,7 +10337,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>30</v>
       </c>
@@ -10309,7 +10363,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>31</v>
       </c>
@@ -10335,7 +10389,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>32</v>
       </c>
@@ -10361,7 +10415,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>33</v>
       </c>
@@ -10387,7 +10441,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>34</v>
       </c>
@@ -10413,7 +10467,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="11">
         <v>35</v>
       </c>
@@ -10439,7 +10493,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>36</v>
       </c>
@@ -10465,7 +10519,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>37</v>
       </c>
@@ -10491,7 +10545,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>38</v>
       </c>
@@ -10517,7 +10571,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>39</v>
       </c>
@@ -10543,7 +10597,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>40</v>
       </c>
@@ -10569,7 +10623,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>41</v>
       </c>
@@ -10595,7 +10649,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>42</v>
       </c>
@@ -10621,7 +10675,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>43</v>
       </c>
@@ -10647,7 +10701,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44</v>
       </c>
@@ -10673,7 +10727,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>45</v>
       </c>
@@ -10699,7 +10753,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>46</v>
       </c>
@@ -10725,7 +10779,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="11">
         <v>47</v>
       </c>
@@ -10751,7 +10805,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>48</v>
       </c>
@@ -10777,7 +10831,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>49</v>
       </c>
@@ -10803,7 +10857,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="11">
         <v>50</v>
       </c>
@@ -10829,7 +10883,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>51</v>
       </c>
@@ -10855,7 +10909,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>52</v>
       </c>
@@ -10881,7 +10935,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>53</v>
       </c>
@@ -10907,7 +10961,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>54</v>
       </c>
@@ -10933,7 +10987,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>55</v>
       </c>
@@ -10959,7 +11013,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>56</v>
       </c>
@@ -10985,7 +11039,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>57</v>
       </c>
@@ -11011,7 +11065,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>58</v>
       </c>
@@ -11037,7 +11091,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>59</v>
       </c>
@@ -11063,12 +11117,12 @@
         <v>598</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B238" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>1071</v>
       </c>
@@ -11094,7 +11148,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>1</v>
       </c>
@@ -11120,7 +11174,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>2</v>
       </c>
@@ -11146,7 +11200,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>3</v>
       </c>
@@ -11172,7 +11226,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>4</v>
       </c>
@@ -11198,7 +11252,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>5</v>
       </c>
@@ -11224,7 +11278,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>6</v>
       </c>
@@ -11250,7 +11304,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>7</v>
       </c>
@@ -11276,7 +11330,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>8</v>
       </c>
@@ -11302,7 +11356,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>9</v>
       </c>
@@ -11328,7 +11382,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>10</v>
       </c>
@@ -11354,7 +11408,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>11</v>
       </c>
@@ -11380,7 +11434,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>12</v>
       </c>
@@ -11406,7 +11460,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>13</v>
       </c>
@@ -11432,7 +11486,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>14</v>
       </c>
@@ -11458,7 +11512,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>15</v>
       </c>
@@ -11484,7 +11538,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>16</v>
       </c>
@@ -11510,7 +11564,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>17</v>
       </c>
@@ -11536,7 +11590,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>18</v>
       </c>
@@ -11562,7 +11616,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>19</v>
       </c>
@@ -11588,7 +11642,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>20</v>
       </c>
@@ -11614,7 +11668,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>21</v>
       </c>
@@ -11640,7 +11694,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>22</v>
       </c>
@@ -11666,7 +11720,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>23</v>
       </c>
@@ -11692,7 +11746,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>24</v>
       </c>
@@ -11718,7 +11772,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>25</v>
       </c>
@@ -11744,7 +11798,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>26</v>
       </c>
@@ -11770,7 +11824,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>27</v>
       </c>
@@ -11796,7 +11850,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>28</v>
       </c>
@@ -11822,7 +11876,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>29</v>
       </c>
@@ -11848,7 +11902,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>30</v>
       </c>
@@ -11874,7 +11928,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>31</v>
       </c>
@@ -11900,7 +11954,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>32</v>
       </c>
@@ -11926,7 +11980,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>33</v>
       </c>
@@ -11952,7 +12006,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>34</v>
       </c>
@@ -11978,12 +12032,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B275" s="3" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
         <v>1071</v>
       </c>
@@ -12009,7 +12063,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>1</v>
       </c>
@@ -12035,7 +12089,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>2</v>
       </c>
@@ -12061,7 +12115,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>3</v>
       </c>
@@ -12087,7 +12141,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>4</v>
       </c>
@@ -12113,7 +12167,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>5</v>
       </c>
@@ -12139,7 +12193,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>6</v>
       </c>
@@ -12165,7 +12219,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>7</v>
       </c>
@@ -12191,7 +12245,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>8</v>
       </c>
@@ -12217,7 +12271,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>9</v>
       </c>
@@ -12243,7 +12297,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>10</v>
       </c>
@@ -12269,7 +12323,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>11</v>
       </c>
@@ -12295,7 +12349,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>12</v>
       </c>
@@ -12321,7 +12375,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>13</v>
       </c>
@@ -12347,7 +12401,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>14</v>
       </c>
@@ -12373,7 +12427,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>15</v>
       </c>
@@ -12399,7 +12453,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>16</v>
       </c>
@@ -12425,7 +12479,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>17</v>
       </c>
@@ -12451,7 +12505,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>18</v>
       </c>
@@ -12477,7 +12531,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>19</v>
       </c>
@@ -12503,7 +12557,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>20</v>
       </c>
@@ -12529,7 +12583,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>21</v>
       </c>
@@ -12555,7 +12609,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>22</v>
       </c>
@@ -12581,7 +12635,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>23</v>
       </c>
@@ -12607,7 +12661,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>24</v>
       </c>
@@ -12633,7 +12687,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>25</v>
       </c>
@@ -12659,7 +12713,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>26</v>
       </c>
@@ -12685,7 +12739,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>27</v>
       </c>
@@ -12711,7 +12765,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>28</v>
       </c>
@@ -12737,7 +12791,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>29</v>
       </c>
@@ -12763,7 +12817,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>30</v>
       </c>
@@ -12789,7 +12843,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>31</v>
       </c>
@@ -12815,7 +12869,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>32</v>
       </c>
@@ -12841,7 +12895,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>33</v>
       </c>
@@ -12867,12 +12921,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B311" s="3" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
         <v>1071</v>
       </c>
@@ -12898,7 +12952,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>1</v>
       </c>
@@ -12924,7 +12978,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>2</v>
       </c>
@@ -12950,7 +13004,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>3</v>
       </c>
@@ -12976,7 +13030,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>4</v>
       </c>
@@ -13002,7 +13056,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>5</v>
       </c>
@@ -13028,7 +13082,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>6</v>
       </c>
@@ -13054,7 +13108,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>7</v>
       </c>
@@ -13080,7 +13134,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>8</v>
       </c>
@@ -13106,7 +13160,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>9</v>
       </c>
@@ -13132,7 +13186,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>10</v>
       </c>
@@ -13158,7 +13212,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>11</v>
       </c>
@@ -13184,7 +13238,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>12</v>
       </c>
@@ -13210,7 +13264,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>13</v>
       </c>
@@ -13236,7 +13290,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>14</v>
       </c>
@@ -13262,7 +13316,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>15</v>
       </c>
@@ -13288,7 +13342,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>16</v>
       </c>
@@ -13314,7 +13368,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>17</v>
       </c>
@@ -13340,7 +13394,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>18</v>
       </c>
@@ -13366,7 +13420,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>19</v>
       </c>
@@ -13392,7 +13446,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>20</v>
       </c>
@@ -13418,7 +13472,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>21</v>
       </c>
@@ -13444,7 +13498,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>22</v>
       </c>
@@ -13470,7 +13524,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>23</v>
       </c>
@@ -13496,7 +13550,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>24</v>
       </c>
@@ -13522,7 +13576,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>25</v>
       </c>
@@ -13548,7 +13602,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>26</v>
       </c>
@@ -13574,7 +13628,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>27</v>
       </c>
@@ -13600,7 +13654,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>28</v>
       </c>
@@ -13626,7 +13680,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>29</v>
       </c>
@@ -13652,7 +13706,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>30</v>
       </c>
@@ -13678,7 +13732,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>31</v>
       </c>
@@ -13704,7 +13758,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>32</v>
       </c>
@@ -13730,7 +13784,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>33</v>
       </c>
@@ -13756,7 +13810,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>34</v>
       </c>
@@ -13782,7 +13836,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>35</v>
       </c>
@@ -13808,7 +13862,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>36</v>
       </c>
@@ -13834,7 +13888,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>37</v>
       </c>
@@ -13860,7 +13914,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>38</v>
       </c>
@@ -13886,7 +13940,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>39</v>
       </c>
@@ -13912,7 +13966,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" s="11">
         <v>40</v>
       </c>
@@ -13938,7 +13992,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" s="11">
         <v>41</v>
       </c>
@@ -13964,7 +14018,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" s="11">
         <v>42</v>
       </c>
@@ -13990,7 +14044,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" s="11">
         <v>43</v>
       </c>
@@ -14016,7 +14070,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356" s="11">
         <v>44</v>
       </c>
@@ -14042,7 +14096,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357" s="11">
         <v>45</v>
       </c>
@@ -14068,7 +14122,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358" s="11">
         <v>46</v>
       </c>
@@ -14094,7 +14148,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" s="11">
         <v>47</v>
       </c>
@@ -14120,7 +14174,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" s="11">
         <v>48</v>
       </c>
@@ -14146,7 +14200,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" s="11">
         <v>49</v>
       </c>
@@ -14172,7 +14226,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" s="11">
         <v>50</v>
       </c>
@@ -14198,7 +14252,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" s="11">
         <v>51</v>
       </c>
@@ -14224,7 +14278,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" s="11">
         <v>52</v>
       </c>
@@ -14250,7 +14304,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" s="11">
         <v>53</v>
       </c>
@@ -14276,7 +14330,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" s="11">
         <v>54</v>
       </c>
@@ -14302,7 +14356,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" s="11">
         <v>55</v>
       </c>
@@ -14328,7 +14382,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" s="11">
         <v>56</v>
       </c>
@@ -14354,7 +14408,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369" s="11">
         <v>57</v>
       </c>
@@ -14380,7 +14434,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" s="11">
         <v>58</v>
       </c>
@@ -14406,7 +14460,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" s="11">
         <v>59</v>
       </c>
@@ -14432,7 +14486,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372" s="11">
         <v>60</v>
       </c>
@@ -14458,7 +14512,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373" s="11">
         <v>61</v>
       </c>
@@ -14484,7 +14538,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374" s="11">
         <v>62</v>
       </c>
@@ -14510,7 +14564,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375" s="11">
         <v>63</v>
       </c>
@@ -14536,7 +14590,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376" s="11">
         <v>64</v>
       </c>
@@ -14562,7 +14616,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377" s="11">
         <v>65</v>
       </c>
@@ -14588,7 +14642,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378" s="11">
         <v>66</v>
       </c>
@@ -14614,7 +14668,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379" s="11">
         <v>67</v>
       </c>
@@ -14640,7 +14694,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380" s="11">
         <v>68</v>
       </c>
@@ -14666,7 +14720,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381" s="11">
         <v>69</v>
       </c>
@@ -14692,7 +14746,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382" s="11">
         <v>70</v>
       </c>
@@ -14718,7 +14772,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383" s="11">
         <v>71</v>
       </c>
@@ -14744,7 +14798,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384" s="11">
         <v>72</v>
       </c>
@@ -14770,7 +14824,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385" s="11">
         <v>73</v>
       </c>
@@ -14796,7 +14850,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386" s="11">
         <v>74</v>
       </c>
@@ -14822,7 +14876,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387" s="11">
         <v>75</v>
       </c>
@@ -14848,7 +14902,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388" s="11">
         <v>76</v>
       </c>
@@ -14874,7 +14928,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389" s="11">
         <v>77</v>
       </c>
@@ -14900,7 +14954,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390" s="11">
         <v>78</v>
       </c>
@@ -14926,7 +14980,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>79</v>
       </c>
@@ -14950,7 +15004,7 @@
       </c>
       <c r="H391" s="1"/>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>80</v>
       </c>
@@ -14974,12 +15028,12 @@
       </c>
       <c r="H392" s="1"/>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B394" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395" s="4" t="s">
         <v>1071</v>
       </c>
@@ -15005,7 +15059,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A396" s="1">
+        <v>1</v>
+      </c>
       <c r="B396" s="1" t="s">
         <v>966</v>
       </c>
@@ -15028,7 +15085,10 @@
         <v>984</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A397" s="1">
+        <v>2</v>
+      </c>
       <c r="B397" s="1" t="s">
         <v>967</v>
       </c>
@@ -15051,7 +15111,10 @@
         <v>984</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A398" s="1">
+        <v>3</v>
+      </c>
       <c r="B398" s="1" t="s">
         <v>968</v>
       </c>
@@ -15074,7 +15137,10 @@
         <v>984</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A399" s="1">
+        <v>4</v>
+      </c>
       <c r="B399" s="1" t="s">
         <v>969</v>
       </c>
@@ -15097,7 +15163,10 @@
         <v>985</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A400" s="1">
+        <v>5</v>
+      </c>
       <c r="B400" s="1" t="s">
         <v>970</v>
       </c>
@@ -15120,7 +15189,10 @@
         <v>476</v>
       </c>
     </row>
-    <row r="401" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A401" s="1">
+        <v>6</v>
+      </c>
       <c r="B401" s="1" t="s">
         <v>971</v>
       </c>
@@ -15143,7 +15215,10 @@
         <v>476</v>
       </c>
     </row>
-    <row r="402" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A402" s="1">
+        <v>7</v>
+      </c>
       <c r="B402" s="1" t="s">
         <v>972</v>
       </c>
@@ -15166,7 +15241,10 @@
         <v>476</v>
       </c>
     </row>
-    <row r="403" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A403" s="1">
+        <v>8</v>
+      </c>
       <c r="B403" s="1" t="s">
         <v>973</v>
       </c>
@@ -15189,7 +15267,10 @@
         <v>986</v>
       </c>
     </row>
-    <row r="404" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A404" s="1">
+        <v>9</v>
+      </c>
       <c r="B404" s="1" t="s">
         <v>974</v>
       </c>
@@ -15212,7 +15293,10 @@
         <v>987</v>
       </c>
     </row>
-    <row r="405" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A405" s="1">
+        <v>10</v>
+      </c>
       <c r="B405" s="1" t="s">
         <v>975</v>
       </c>
@@ -15235,7 +15319,10 @@
         <v>988</v>
       </c>
     </row>
-    <row r="406" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A406" s="1">
+        <v>11</v>
+      </c>
       <c r="B406" s="1" t="s">
         <v>976</v>
       </c>
@@ -15258,7 +15345,10 @@
         <v>989</v>
       </c>
     </row>
-    <row r="407" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A407" s="1">
+        <v>12</v>
+      </c>
       <c r="B407" s="1" t="s">
         <v>977</v>
       </c>
@@ -15281,7 +15371,10 @@
         <v>990</v>
       </c>
     </row>
-    <row r="408" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A408" s="1">
+        <v>13</v>
+      </c>
       <c r="B408" s="1" t="s">
         <v>978</v>
       </c>
@@ -15304,7 +15397,10 @@
         <v>991</v>
       </c>
     </row>
-    <row r="409" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A409" s="1">
+        <v>14</v>
+      </c>
       <c r="B409" s="1" t="s">
         <v>979</v>
       </c>
@@ -15327,7 +15423,10 @@
         <v>992</v>
       </c>
     </row>
-    <row r="410" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A410" s="1">
+        <v>15</v>
+      </c>
       <c r="B410" s="1" t="s">
         <v>980</v>
       </c>
@@ -15350,7 +15449,10 @@
         <v>992</v>
       </c>
     </row>
-    <row r="411" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A411" s="1">
+        <v>16</v>
+      </c>
       <c r="B411" s="1" t="s">
         <v>981</v>
       </c>
@@ -15373,7 +15475,10 @@
         <v>991</v>
       </c>
     </row>
-    <row r="412" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A412" s="1">
+        <v>17</v>
+      </c>
       <c r="B412" s="1" t="s">
         <v>982</v>
       </c>
@@ -15396,7 +15501,10 @@
         <v>991</v>
       </c>
     </row>
-    <row r="413" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A413" s="1">
+        <v>18</v>
+      </c>
       <c r="B413" s="1" t="s">
         <v>983</v>
       </c>
@@ -15419,288 +15527,324 @@
         <v>991</v>
       </c>
     </row>
-    <row r="414" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B414" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="C414" s="1" t="s">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A414" s="11">
+        <v>19</v>
+      </c>
+      <c r="B414" s="11" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C414" s="11" t="s">
         <v>1003</v>
       </c>
-      <c r="D414" s="1" t="s">
+      <c r="D414" s="11" t="s">
         <v>1029</v>
       </c>
-      <c r="E414" s="1" t="s">
+      <c r="E414" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F414" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G414" s="1">
+      <c r="F414" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G414" s="11">
         <v>1</v>
       </c>
-      <c r="H414" s="1" t="s">
+      <c r="H414" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="415" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B415" s="1" t="s">
-        <v>967</v>
-      </c>
-      <c r="C415" s="1" t="s">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A415" s="11">
+        <v>20</v>
+      </c>
+      <c r="B415" s="11" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C415" s="11" t="s">
         <v>1005</v>
       </c>
-      <c r="D415" s="1" t="s">
+      <c r="D415" s="11" t="s">
         <v>1030</v>
       </c>
-      <c r="E415" s="1" t="s">
+      <c r="E415" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F415" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G415" s="1">
+      <c r="F415" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G415" s="11">
         <v>1</v>
       </c>
-      <c r="H415" s="1" t="s">
+      <c r="H415" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="416" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B416" s="1" t="s">
-        <v>968</v>
-      </c>
-      <c r="C416" s="1" t="s">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A416" s="11">
+        <v>21</v>
+      </c>
+      <c r="B416" s="11" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C416" s="11" t="s">
         <v>1007</v>
       </c>
-      <c r="D416" s="1" t="s">
+      <c r="D416" s="11" t="s">
         <v>1031</v>
       </c>
-      <c r="E416" s="1" t="s">
+      <c r="E416" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F416" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G416" s="1">
+      <c r="F416" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G416" s="11">
         <v>1</v>
       </c>
-      <c r="H416" s="1" t="s">
+      <c r="H416" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B417" s="1" t="s">
-        <v>969</v>
-      </c>
-      <c r="C417" s="1" t="s">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A417" s="11">
+        <v>22</v>
+      </c>
+      <c r="B417" s="11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C417" s="11" t="s">
         <v>1008</v>
       </c>
-      <c r="D417" s="1" t="s">
+      <c r="D417" s="11" t="s">
         <v>1032</v>
       </c>
-      <c r="E417" s="1" t="s">
+      <c r="E417" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F417" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G417" s="1">
+      <c r="F417" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G417" s="11">
         <v>1</v>
       </c>
-      <c r="H417" s="1" t="s">
+      <c r="H417" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B418" s="1" t="s">
-        <v>970</v>
-      </c>
-      <c r="C418" s="1" t="s">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A418" s="11">
+        <v>23</v>
+      </c>
+      <c r="B418" s="11" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C418" s="11" t="s">
         <v>1009</v>
       </c>
-      <c r="D418" s="1" t="s">
+      <c r="D418" s="11" t="s">
         <v>1033</v>
       </c>
-      <c r="E418" s="1" t="s">
+      <c r="E418" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F418" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G418" s="1">
+      <c r="F418" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G418" s="11">
         <v>1</v>
       </c>
-      <c r="H418" s="1" t="s">
+      <c r="H418" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B419" s="1" t="s">
-        <v>971</v>
-      </c>
-      <c r="C419" s="1" t="s">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A419" s="11">
+        <v>24</v>
+      </c>
+      <c r="B419" s="11" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C419" s="11" t="s">
         <v>1010</v>
       </c>
-      <c r="D419" s="1" t="s">
+      <c r="D419" s="11" t="s">
         <v>1034</v>
       </c>
-      <c r="E419" s="1" t="s">
+      <c r="E419" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F419" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G419" s="1">
+      <c r="F419" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G419" s="11">
         <v>1</v>
       </c>
-      <c r="H419" s="1" t="s">
+      <c r="H419" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B420" s="1" t="s">
-        <v>972</v>
-      </c>
-      <c r="C420" s="1" t="s">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A420" s="11">
+        <v>25</v>
+      </c>
+      <c r="B420" s="11" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C420" s="11" t="s">
         <v>1011</v>
       </c>
-      <c r="D420" s="1" t="s">
+      <c r="D420" s="11" t="s">
         <v>1035</v>
       </c>
-      <c r="E420" s="1" t="s">
+      <c r="E420" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F420" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G420" s="1">
+      <c r="F420" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G420" s="11">
         <v>1</v>
       </c>
-      <c r="H420" s="1" t="s">
+      <c r="H420" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B421" s="1" t="s">
-        <v>973</v>
-      </c>
-      <c r="C421" s="1" t="s">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A421" s="11">
+        <v>26</v>
+      </c>
+      <c r="B421" s="11" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C421" s="11" t="s">
         <v>1012</v>
       </c>
-      <c r="D421" s="1" t="s">
+      <c r="D421" s="11" t="s">
         <v>1036</v>
       </c>
-      <c r="E421" s="1" t="s">
+      <c r="E421" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F421" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G421" s="1">
+      <c r="F421" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G421" s="11">
         <v>1</v>
       </c>
-      <c r="H421" s="1" t="s">
+      <c r="H421" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B422" s="1" t="s">
-        <v>974</v>
-      </c>
-      <c r="C422" s="1" t="s">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A422" s="11">
+        <v>27</v>
+      </c>
+      <c r="B422" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C422" s="11" t="s">
         <v>1013</v>
       </c>
-      <c r="D422" s="1" t="s">
+      <c r="D422" s="11" t="s">
         <v>1037</v>
       </c>
-      <c r="E422" s="1" t="s">
+      <c r="E422" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F422" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G422" s="1">
+      <c r="F422" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G422" s="11">
         <v>1</v>
       </c>
-      <c r="H422" s="1" t="s">
+      <c r="H422" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B423" s="1" t="s">
-        <v>975</v>
-      </c>
-      <c r="C423" s="1" t="s">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A423" s="11">
+        <v>28</v>
+      </c>
+      <c r="B423" s="11" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C423" s="11" t="s">
         <v>1014</v>
       </c>
-      <c r="D423" s="1" t="s">
+      <c r="D423" s="11" t="s">
         <v>1038</v>
       </c>
-      <c r="E423" s="1" t="s">
+      <c r="E423" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F423" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G423" s="1">
+      <c r="F423" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G423" s="11">
         <v>1</v>
       </c>
-      <c r="H423" s="1" t="s">
+      <c r="H423" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B424" s="1" t="s">
-        <v>976</v>
-      </c>
-      <c r="C424" s="1" t="s">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A424" s="11">
+        <v>29</v>
+      </c>
+      <c r="B424" s="11" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C424" s="11" t="s">
         <v>1015</v>
       </c>
-      <c r="D424" s="1" t="s">
+      <c r="D424" s="11" t="s">
         <v>1039</v>
       </c>
-      <c r="E424" s="1" t="s">
+      <c r="E424" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F424" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G424" s="1">
+      <c r="F424" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G424" s="11">
         <v>1</v>
       </c>
-      <c r="H424" s="1" t="s">
+      <c r="H424" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B425" s="1" t="s">
-        <v>977</v>
-      </c>
-      <c r="C425" s="1" t="s">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A425" s="11">
+        <v>30</v>
+      </c>
+      <c r="B425" s="11" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C425" s="11" t="s">
         <v>1016</v>
       </c>
-      <c r="D425" s="1" t="s">
+      <c r="D425" s="11" t="s">
         <v>1040</v>
       </c>
-      <c r="E425" s="1" t="s">
+      <c r="E425" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F425" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G425" s="1">
+      <c r="F425" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G425" s="11">
         <v>1</v>
       </c>
-      <c r="H425" s="1" t="s">
+      <c r="H425" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B427" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A428" s="4" t="s">
         <v>1071</v>
       </c>
@@ -15726,7 +15870,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A429" s="1">
+        <v>1</v>
+      </c>
       <c r="B429" s="1" t="s">
         <v>993</v>
       </c>
@@ -15749,7 +15896,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A430" s="1">
+        <v>2</v>
+      </c>
       <c r="B430" s="1" t="s">
         <v>994</v>
       </c>
@@ -15772,7 +15922,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A431" s="1">
+        <v>3</v>
+      </c>
       <c r="B431" s="1" t="s">
         <v>995</v>
       </c>
@@ -15795,7 +15948,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A432" s="1">
+        <v>4</v>
+      </c>
       <c r="B432" s="1" t="s">
         <v>996</v>
       </c>
@@ -15818,7 +15974,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="433" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A433" s="1">
+        <v>5</v>
+      </c>
       <c r="B433" s="1" t="s">
         <v>997</v>
       </c>
@@ -15841,7 +16000,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="434" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A434" s="1">
+        <v>6</v>
+      </c>
       <c r="B434" s="1" t="s">
         <v>998</v>
       </c>
@@ -15864,7 +16026,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="435" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A435" s="1">
+        <v>7</v>
+      </c>
       <c r="B435" s="1" t="s">
         <v>999</v>
       </c>
@@ -15887,7 +16052,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="436" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A436" s="1">
+        <v>8</v>
+      </c>
       <c r="B436" s="1" t="s">
         <v>1000</v>
       </c>
@@ -15910,7 +16078,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="437" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A437" s="1">
+        <v>9</v>
+      </c>
       <c r="B437" s="1" t="s">
         <v>1001</v>
       </c>
@@ -15933,7 +16104,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="438" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A438" s="1">
+        <v>10</v>
+      </c>
       <c r="B438" s="1" t="s">
         <v>1002</v>
       </c>

</xml_diff>

<commit_message>
Update CSV for import DB
</commit_message>
<xml_diff>
--- a/dataset_competition/META_DATA.xlsx
+++ b/dataset_competition/META_DATA.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seolab/bro.py/dataset_competition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SERVER1\bro.py\dataset_competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="460" windowWidth="22380" windowHeight="14760" tabRatio="681" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="2715" yWindow="465" windowWidth="22380" windowHeight="14760" tabRatio="681" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="테이블" sheetId="2" r:id="rId1"/>
@@ -31,21 +31,18 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="1142">
   <si>
     <t>SPX</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3622,6 +3619,10 @@
   </si>
   <si>
     <t>arKOFXINDD_YoY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aJPCBLD_YoY</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3630,10 +3631,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -4153,8 +4154,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4185,8 +4186,8 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4306,15 +4307,6 @@
     <cellStyle name="60% - Accent4" xfId="18"/>
     <cellStyle name="60% - Accent5" xfId="19"/>
     <cellStyle name="60% - Accent6" xfId="20"/>
-    <cellStyle name="기본" xfId="0" builtinId="0"/>
-    <cellStyle name="백분율 2" xfId="53"/>
-    <cellStyle name="스타일 1" xfId="2"/>
-    <cellStyle name="콤마 [0]_일일금융시장_new" xfId="21"/>
-    <cellStyle name="콤마_일일금융시장_new" xfId="22"/>
-    <cellStyle name="표준 2" xfId="23"/>
-    <cellStyle name="표준 3" xfId="54"/>
-    <cellStyle name="표준 4" xfId="1"/>
-    <cellStyle name="하이퍼링크" xfId="55" builtinId="8"/>
     <cellStyle name="Accent1" xfId="24"/>
     <cellStyle name="Accent2" xfId="25"/>
     <cellStyle name="Accent3" xfId="26"/>
@@ -4344,6 +4336,15 @@
     <cellStyle name="Title" xfId="50"/>
     <cellStyle name="Total" xfId="51"/>
     <cellStyle name="Warning Text" xfId="52"/>
+    <cellStyle name="백분율 2" xfId="53"/>
+    <cellStyle name="스타일 1" xfId="2"/>
+    <cellStyle name="콤마 [0]_일일금융시장_new" xfId="21"/>
+    <cellStyle name="콤마_일일금융시장_new" xfId="22"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="23"/>
+    <cellStyle name="표준 3" xfId="54"/>
+    <cellStyle name="표준 4" xfId="1"/>
+    <cellStyle name="하이퍼링크" xfId="55" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4625,14 +4626,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
     <col min="2" max="3" width="29.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -4649,7 +4650,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -4717,7 +4718,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1063</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1064</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1065</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>100</v>
       </c>
@@ -4785,7 +4786,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>495</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>496</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>494</v>
       </c>
@@ -4836,7 +4837,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>498</v>
       </c>
@@ -4853,7 +4854,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>497</v>
       </c>
@@ -4870,7 +4871,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>500</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>499</v>
       </c>
@@ -4904,7 +4905,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>501</v>
       </c>
@@ -4946,13 +4947,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="29.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>258</v>
       </c>
@@ -4960,7 +4961,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4968,7 +4969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +4977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4984,7 +4985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -4992,7 +4993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5000,7 +5001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -5016,7 +5017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -5024,7 +5025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -5040,7 +5041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -5060,13 +5061,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="29.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>258</v>
       </c>
@@ -5074,7 +5075,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -5082,7 +5083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5090,7 +5091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -5098,7 +5099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -5106,7 +5107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5114,7 +5115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5132,27 +5133,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G423" sqref="D1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A275" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="4" width="36.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="22.375" customWidth="1"/>
+    <col min="3" max="4" width="36.125" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="10.875" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1071</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5204,7 +5205,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5256,7 +5257,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5282,7 +5283,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5308,7 +5309,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5334,7 +5335,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5386,7 +5387,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5412,7 +5413,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -5464,7 +5465,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -5490,7 +5491,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -5516,7 +5517,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5542,7 +5543,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5594,7 +5595,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5620,7 +5621,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -5646,7 +5647,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5672,7 +5673,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -5698,7 +5699,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -5724,7 +5725,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -5750,7 +5751,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -5776,7 +5777,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -5802,7 +5803,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -5828,7 +5829,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -5880,7 +5881,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -5906,7 +5907,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -5932,7 +5933,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -5958,12 +5959,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>1070</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>1071</v>
       </c>
@@ -5989,7 +5990,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1</v>
       </c>
@@ -6015,7 +6016,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -6041,7 +6042,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>3</v>
       </c>
@@ -6067,7 +6068,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>4</v>
       </c>
@@ -6093,7 +6094,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>5</v>
       </c>
@@ -6119,7 +6120,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>6</v>
       </c>
@@ -6145,7 +6146,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>7</v>
       </c>
@@ -6171,7 +6172,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>8</v>
       </c>
@@ -6197,7 +6198,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>9</v>
       </c>
@@ -6223,7 +6224,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>10</v>
       </c>
@@ -6249,7 +6250,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>11</v>
       </c>
@@ -6275,7 +6276,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>12</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>13</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>14</v>
       </c>
@@ -6353,7 +6354,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>15</v>
       </c>
@@ -6379,7 +6380,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>16</v>
       </c>
@@ -6405,7 +6406,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
         <v>17</v>
       </c>
@@ -6431,7 +6432,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>18</v>
       </c>
@@ -6457,7 +6458,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>19</v>
       </c>
@@ -6483,7 +6484,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>20</v>
       </c>
@@ -6509,7 +6510,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>21</v>
       </c>
@@ -6535,7 +6536,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>22</v>
       </c>
@@ -6561,7 +6562,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>23</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>24</v>
       </c>
@@ -6613,7 +6614,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>25</v>
       </c>
@@ -6639,7 +6640,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>26</v>
       </c>
@@ -6665,7 +6666,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>27</v>
       </c>
@@ -6691,7 +6692,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>28</v>
       </c>
@@ -6717,7 +6718,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>29</v>
       </c>
@@ -6743,7 +6744,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>30</v>
       </c>
@@ -6769,7 +6770,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="10">
         <v>31</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="10">
         <v>32</v>
       </c>
@@ -6821,7 +6822,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="10">
         <v>33</v>
       </c>
@@ -6847,7 +6848,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="10">
         <v>34</v>
       </c>
@@ -6873,7 +6874,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="10">
         <v>35</v>
       </c>
@@ -6899,7 +6900,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>36</v>
       </c>
@@ -6925,7 +6926,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="11">
         <v>37</v>
       </c>
@@ -6951,7 +6952,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>38</v>
       </c>
@@ -6977,7 +6978,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>39</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>40</v>
       </c>
@@ -7029,7 +7030,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>41</v>
       </c>
@@ -7055,7 +7056,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>42</v>
       </c>
@@ -7081,7 +7082,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>43</v>
       </c>
@@ -7107,7 +7108,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>44</v>
       </c>
@@ -7133,7 +7134,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>45</v>
       </c>
@@ -7159,7 +7160,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>46</v>
       </c>
@@ -7185,7 +7186,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>47</v>
       </c>
@@ -7211,7 +7212,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>48</v>
       </c>
@@ -7237,7 +7238,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>49</v>
       </c>
@@ -7263,7 +7264,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>50</v>
       </c>
@@ -7289,7 +7290,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>51</v>
       </c>
@@ -7315,7 +7316,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>52</v>
       </c>
@@ -7341,7 +7342,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>53</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>54</v>
       </c>
@@ -7393,7 +7394,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>55</v>
       </c>
@@ -7419,7 +7420,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>56</v>
       </c>
@@ -7445,7 +7446,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>57</v>
       </c>
@@ -7471,7 +7472,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>58</v>
       </c>
@@ -7497,12 +7498,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>1071</v>
       </c>
@@ -7528,7 +7529,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>1</v>
       </c>
@@ -7554,7 +7555,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>2</v>
       </c>
@@ -7580,7 +7581,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>3</v>
       </c>
@@ -7606,7 +7607,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>4</v>
       </c>
@@ -7632,7 +7633,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>5</v>
       </c>
@@ -7658,7 +7659,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>6</v>
       </c>
@@ -7684,7 +7685,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <v>7</v>
       </c>
@@ -7710,7 +7711,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>8</v>
       </c>
@@ -7736,7 +7737,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>9</v>
       </c>
@@ -7762,7 +7763,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>10</v>
       </c>
@@ -7788,7 +7789,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>11</v>
       </c>
@@ -7814,7 +7815,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>12</v>
       </c>
@@ -7840,7 +7841,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>13</v>
       </c>
@@ -7866,7 +7867,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>14</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>15</v>
       </c>
@@ -7918,7 +7919,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>16</v>
       </c>
@@ -7944,7 +7945,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="10">
         <v>17</v>
       </c>
@@ -7970,7 +7971,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>18</v>
       </c>
@@ -7996,7 +7997,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>19</v>
       </c>
@@ -8022,7 +8023,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>20</v>
       </c>
@@ -8048,7 +8049,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>21</v>
       </c>
@@ -8074,7 +8075,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>22</v>
       </c>
@@ -8100,7 +8101,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>23</v>
       </c>
@@ -8126,7 +8127,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>24</v>
       </c>
@@ -8152,7 +8153,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>25</v>
       </c>
@@ -8178,7 +8179,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>26</v>
       </c>
@@ -8204,7 +8205,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>27</v>
       </c>
@@ -8230,7 +8231,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>28</v>
       </c>
@@ -8256,7 +8257,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>29</v>
       </c>
@@ -8282,7 +8283,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>30</v>
       </c>
@@ -8308,7 +8309,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>31</v>
       </c>
@@ -8334,7 +8335,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>32</v>
       </c>
@@ -8360,7 +8361,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>33</v>
       </c>
@@ -8386,7 +8387,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>34</v>
       </c>
@@ -8412,7 +8413,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>35</v>
       </c>
@@ -8438,7 +8439,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>36</v>
       </c>
@@ -8464,7 +8465,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>37</v>
       </c>
@@ -8490,7 +8491,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>38</v>
       </c>
@@ -8516,7 +8517,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
         <v>39</v>
       </c>
@@ -8542,7 +8543,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="11">
         <v>40</v>
       </c>
@@ -8568,7 +8569,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>41</v>
       </c>
@@ -8594,7 +8595,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>42</v>
       </c>
@@ -8620,7 +8621,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>43</v>
       </c>
@@ -8646,7 +8647,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>44</v>
       </c>
@@ -8672,7 +8673,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>45</v>
       </c>
@@ -8698,7 +8699,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>46</v>
       </c>
@@ -8724,7 +8725,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>47</v>
       </c>
@@ -8750,7 +8751,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>48</v>
       </c>
@@ -8776,7 +8777,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>49</v>
       </c>
@@ -8802,7 +8803,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>50</v>
       </c>
@@ -8828,7 +8829,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>51</v>
       </c>
@@ -8854,7 +8855,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>52</v>
       </c>
@@ -8880,7 +8881,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>53</v>
       </c>
@@ -8906,7 +8907,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>54</v>
       </c>
@@ -8932,7 +8933,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>55</v>
       </c>
@@ -8958,7 +8959,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>56</v>
       </c>
@@ -8984,7 +8985,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>57</v>
       </c>
@@ -9010,7 +9011,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>58</v>
       </c>
@@ -9036,7 +9037,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>59</v>
       </c>
@@ -9062,7 +9063,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>60</v>
       </c>
@@ -9088,7 +9089,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>61</v>
       </c>
@@ -9114,7 +9115,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>62</v>
       </c>
@@ -9140,7 +9141,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>63</v>
       </c>
@@ -9166,7 +9167,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="11">
         <v>64</v>
       </c>
@@ -9192,7 +9193,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>65</v>
       </c>
@@ -9218,7 +9219,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>66</v>
       </c>
@@ -9244,7 +9245,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="11">
         <v>67</v>
       </c>
@@ -9270,7 +9271,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>68</v>
       </c>
@@ -9296,7 +9297,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="11">
         <v>69</v>
       </c>
@@ -9322,7 +9323,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>70</v>
       </c>
@@ -9348,7 +9349,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>71</v>
       </c>
@@ -9374,7 +9375,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>72</v>
       </c>
@@ -9400,7 +9401,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>73</v>
       </c>
@@ -9426,7 +9427,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>74</v>
       </c>
@@ -9452,7 +9453,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>75</v>
       </c>
@@ -9476,7 +9477,7 @@
       </c>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>76</v>
       </c>
@@ -9500,7 +9501,7 @@
       </c>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>77</v>
       </c>
@@ -9526,7 +9527,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>78</v>
       </c>
@@ -9552,12 +9553,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B176" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>1071</v>
       </c>
@@ -9583,7 +9584,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>1</v>
       </c>
@@ -9609,7 +9610,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" s="11">
         <v>2</v>
       </c>
@@ -9635,7 +9636,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>3</v>
       </c>
@@ -9661,7 +9662,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>4</v>
       </c>
@@ -9687,7 +9688,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>5</v>
       </c>
@@ -9713,7 +9714,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>6</v>
       </c>
@@ -9739,7 +9740,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>7</v>
       </c>
@@ -9765,7 +9766,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>8</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="11">
         <v>9</v>
       </c>
@@ -9817,7 +9818,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>10</v>
       </c>
@@ -9843,7 +9844,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>11</v>
       </c>
@@ -9869,7 +9870,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>12</v>
       </c>
@@ -9895,7 +9896,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>13</v>
       </c>
@@ -9921,7 +9922,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>14</v>
       </c>
@@ -9947,7 +9948,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>15</v>
       </c>
@@ -9973,7 +9974,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>16</v>
       </c>
@@ -9999,7 +10000,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>17</v>
       </c>
@@ -10025,7 +10026,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>18</v>
       </c>
@@ -10051,7 +10052,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" s="11">
         <v>19</v>
       </c>
@@ -10077,7 +10078,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>20</v>
       </c>
@@ -10103,7 +10104,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>21</v>
       </c>
@@ -10129,7 +10130,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>22</v>
       </c>
@@ -10155,7 +10156,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>23</v>
       </c>
@@ -10181,7 +10182,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>24</v>
       </c>
@@ -10207,7 +10208,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>25</v>
       </c>
@@ -10233,7 +10234,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>26</v>
       </c>
@@ -10259,7 +10260,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>27</v>
       </c>
@@ -10285,7 +10286,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>28</v>
       </c>
@@ -10311,7 +10312,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>29</v>
       </c>
@@ -10337,7 +10338,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>30</v>
       </c>
@@ -10363,7 +10364,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>31</v>
       </c>
@@ -10389,7 +10390,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>32</v>
       </c>
@@ -10415,7 +10416,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>33</v>
       </c>
@@ -10441,7 +10442,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>34</v>
       </c>
@@ -10467,7 +10468,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" s="11">
         <v>35</v>
       </c>
@@ -10493,7 +10494,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>36</v>
       </c>
@@ -10519,7 +10520,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>37</v>
       </c>
@@ -10545,7 +10546,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>38</v>
       </c>
@@ -10571,7 +10572,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>39</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>40</v>
       </c>
@@ -10623,7 +10624,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>41</v>
       </c>
@@ -10649,7 +10650,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>42</v>
       </c>
@@ -10675,7 +10676,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>43</v>
       </c>
@@ -10701,7 +10702,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>44</v>
       </c>
@@ -10727,7 +10728,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>45</v>
       </c>
@@ -10753,7 +10754,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>46</v>
       </c>
@@ -10779,7 +10780,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" s="11">
         <v>47</v>
       </c>
@@ -10805,7 +10806,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>48</v>
       </c>
@@ -10831,7 +10832,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>49</v>
       </c>
@@ -10857,7 +10858,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" s="11">
         <v>50</v>
       </c>
@@ -10883,7 +10884,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>51</v>
       </c>
@@ -10909,7 +10910,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>52</v>
       </c>
@@ -10935,7 +10936,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>53</v>
       </c>
@@ -10961,7 +10962,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>54</v>
       </c>
@@ -10987,7 +10988,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>55</v>
       </c>
@@ -11013,7 +11014,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>56</v>
       </c>
@@ -11039,7 +11040,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>57</v>
       </c>
@@ -11065,7 +11066,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>58</v>
       </c>
@@ -11091,7 +11092,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>59</v>
       </c>
@@ -11117,12 +11118,12 @@
         <v>598</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B238" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" s="4" t="s">
         <v>1071</v>
       </c>
@@ -11148,7 +11149,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>1</v>
       </c>
@@ -11174,7 +11175,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>2</v>
       </c>
@@ -11200,7 +11201,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>3</v>
       </c>
@@ -11226,7 +11227,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>4</v>
       </c>
@@ -11252,7 +11253,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>5</v>
       </c>
@@ -11278,7 +11279,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>6</v>
       </c>
@@ -11304,7 +11305,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>7</v>
       </c>
@@ -11330,7 +11331,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>8</v>
       </c>
@@ -11356,7 +11357,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>9</v>
       </c>
@@ -11382,7 +11383,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>10</v>
       </c>
@@ -11408,7 +11409,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>11</v>
       </c>
@@ -11434,7 +11435,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>12</v>
       </c>
@@ -11460,7 +11461,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>13</v>
       </c>
@@ -11486,7 +11487,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>14</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>15</v>
       </c>
@@ -11538,7 +11539,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>16</v>
       </c>
@@ -11564,7 +11565,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>17</v>
       </c>
@@ -11590,7 +11591,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>18</v>
       </c>
@@ -11616,7 +11617,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>19</v>
       </c>
@@ -11642,7 +11643,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>20</v>
       </c>
@@ -11668,7 +11669,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>21</v>
       </c>
@@ -11694,7 +11695,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>22</v>
       </c>
@@ -11720,7 +11721,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>23</v>
       </c>
@@ -11746,7 +11747,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>24</v>
       </c>
@@ -11772,7 +11773,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>25</v>
       </c>
@@ -11798,7 +11799,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>26</v>
       </c>
@@ -11824,7 +11825,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>27</v>
       </c>
@@ -11850,7 +11851,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>28</v>
       </c>
@@ -11876,7 +11877,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>29</v>
       </c>
@@ -11902,7 +11903,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>30</v>
       </c>
@@ -11928,7 +11929,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>31</v>
       </c>
@@ -11954,7 +11955,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>32</v>
       </c>
@@ -11980,7 +11981,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>33</v>
       </c>
@@ -12006,7 +12007,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>34</v>
       </c>
@@ -12032,12 +12033,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B275" s="3" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
         <v>1071</v>
       </c>
@@ -12063,7 +12064,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>1</v>
       </c>
@@ -12089,7 +12090,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>2</v>
       </c>
@@ -12115,7 +12116,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>3</v>
       </c>
@@ -12141,7 +12142,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>4</v>
       </c>
@@ -12167,7 +12168,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>5</v>
       </c>
@@ -12193,7 +12194,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>6</v>
       </c>
@@ -12219,7 +12220,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>7</v>
       </c>
@@ -12245,7 +12246,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>8</v>
       </c>
@@ -12271,7 +12272,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>9</v>
       </c>
@@ -12297,7 +12298,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>10</v>
       </c>
@@ -12323,7 +12324,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>11</v>
       </c>
@@ -12349,7 +12350,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <v>12</v>
       </c>
@@ -12375,7 +12376,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>13</v>
       </c>
@@ -12401,33 +12402,33 @@
         <v>732</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A290" s="1">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A290" s="11">
         <v>14</v>
       </c>
-      <c r="B290" s="1" t="s">
+      <c r="B290" s="11" t="s">
         <v>781</v>
       </c>
-      <c r="C290" s="1" t="s">
+      <c r="C290" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="D290" s="1" t="s">
+      <c r="D290" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="E290" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F290" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G290" s="1">
-        <v>0</v>
-      </c>
-      <c r="H290" s="1" t="s">
+      <c r="E290" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F290" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G290" s="11">
+        <v>0</v>
+      </c>
+      <c r="H290" s="11" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>15</v>
       </c>
@@ -12453,7 +12454,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>16</v>
       </c>
@@ -12479,7 +12480,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>17</v>
       </c>
@@ -12505,7 +12506,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>18</v>
       </c>
@@ -12531,7 +12532,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>19</v>
       </c>
@@ -12557,7 +12558,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>20</v>
       </c>
@@ -12583,7 +12584,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>21</v>
       </c>
@@ -12609,7 +12610,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>22</v>
       </c>
@@ -12635,7 +12636,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>23</v>
       </c>
@@ -12661,7 +12662,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>24</v>
       </c>
@@ -12687,7 +12688,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>25</v>
       </c>
@@ -12713,7 +12714,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>26</v>
       </c>
@@ -12739,7 +12740,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>27</v>
       </c>
@@ -12765,7 +12766,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>28</v>
       </c>
@@ -12791,7 +12792,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>29</v>
       </c>
@@ -12817,7 +12818,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>30</v>
       </c>
@@ -12843,7 +12844,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>31</v>
       </c>
@@ -12869,7 +12870,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>32</v>
       </c>
@@ -12895,38 +12896,38 @@
         <v>249</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A309" s="1">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A309" s="11">
         <v>33</v>
       </c>
-      <c r="B309" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="C309" s="1" t="s">
+      <c r="B309" s="11" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C309" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="D309" s="1" t="s">
+      <c r="D309" s="11" t="s">
         <v>767</v>
       </c>
-      <c r="E309" s="1" t="s">
+      <c r="E309" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F309" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G309" s="1">
-        <v>0</v>
-      </c>
-      <c r="H309" s="1" t="s">
+      <c r="F309" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G309" s="11">
+        <v>0</v>
+      </c>
+      <c r="H309" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B311" s="3" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A312" s="4" t="s">
         <v>1071</v>
       </c>
@@ -12952,7 +12953,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>1</v>
       </c>
@@ -12978,7 +12979,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>2</v>
       </c>
@@ -13004,7 +13005,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>3</v>
       </c>
@@ -13030,7 +13031,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>4</v>
       </c>
@@ -13056,7 +13057,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>5</v>
       </c>
@@ -13082,7 +13083,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>6</v>
       </c>
@@ -13108,7 +13109,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>7</v>
       </c>
@@ -13134,7 +13135,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>8</v>
       </c>
@@ -13160,7 +13161,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>9</v>
       </c>
@@ -13186,7 +13187,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>10</v>
       </c>
@@ -13212,7 +13213,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>11</v>
       </c>
@@ -13238,7 +13239,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>12</v>
       </c>
@@ -13264,7 +13265,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>13</v>
       </c>
@@ -13290,7 +13291,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>14</v>
       </c>
@@ -13316,7 +13317,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>15</v>
       </c>
@@ -13342,7 +13343,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>16</v>
       </c>
@@ -13368,7 +13369,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A329" s="1">
         <v>17</v>
       </c>
@@ -13394,7 +13395,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>18</v>
       </c>
@@ -13420,7 +13421,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>19</v>
       </c>
@@ -13446,7 +13447,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A332" s="1">
         <v>20</v>
       </c>
@@ -13472,7 +13473,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A333" s="1">
         <v>21</v>
       </c>
@@ -13498,7 +13499,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A334" s="1">
         <v>22</v>
       </c>
@@ -13524,7 +13525,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A335" s="1">
         <v>23</v>
       </c>
@@ -13550,7 +13551,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>24</v>
       </c>
@@ -13576,7 +13577,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A337" s="1">
         <v>25</v>
       </c>
@@ -13602,7 +13603,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A338" s="1">
         <v>26</v>
       </c>
@@ -13628,7 +13629,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A339" s="1">
         <v>27</v>
       </c>
@@ -13654,7 +13655,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A340" s="1">
         <v>28</v>
       </c>
@@ -13680,7 +13681,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A341" s="1">
         <v>29</v>
       </c>
@@ -13706,7 +13707,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A342" s="1">
         <v>30</v>
       </c>
@@ -13732,7 +13733,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A343" s="1">
         <v>31</v>
       </c>
@@ -13758,7 +13759,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A344" s="1">
         <v>32</v>
       </c>
@@ -13784,7 +13785,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A345" s="1">
         <v>33</v>
       </c>
@@ -13810,7 +13811,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A346" s="1">
         <v>34</v>
       </c>
@@ -13836,7 +13837,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A347" s="1">
         <v>35</v>
       </c>
@@ -13862,7 +13863,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A348" s="1">
         <v>36</v>
       </c>
@@ -13888,7 +13889,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>37</v>
       </c>
@@ -13914,7 +13915,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A350" s="1">
         <v>38</v>
       </c>
@@ -13940,7 +13941,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A351" s="1">
         <v>39</v>
       </c>
@@ -13966,7 +13967,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A352" s="11">
         <v>40</v>
       </c>
@@ -13992,7 +13993,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A353" s="11">
         <v>41</v>
       </c>
@@ -14018,7 +14019,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A354" s="11">
         <v>42</v>
       </c>
@@ -14044,7 +14045,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A355" s="11">
         <v>43</v>
       </c>
@@ -14070,7 +14071,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A356" s="11">
         <v>44</v>
       </c>
@@ -14096,7 +14097,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A357" s="11">
         <v>45</v>
       </c>
@@ -14122,7 +14123,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A358" s="11">
         <v>46</v>
       </c>
@@ -14148,7 +14149,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A359" s="11">
         <v>47</v>
       </c>
@@ -14174,7 +14175,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A360" s="11">
         <v>48</v>
       </c>
@@ -14200,7 +14201,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A361" s="11">
         <v>49</v>
       </c>
@@ -14226,7 +14227,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A362" s="11">
         <v>50</v>
       </c>
@@ -14252,7 +14253,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A363" s="11">
         <v>51</v>
       </c>
@@ -14278,7 +14279,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A364" s="11">
         <v>52</v>
       </c>
@@ -14304,7 +14305,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A365" s="11">
         <v>53</v>
       </c>
@@ -14330,7 +14331,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A366" s="11">
         <v>54</v>
       </c>
@@ -14356,7 +14357,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A367" s="11">
         <v>55</v>
       </c>
@@ -14382,7 +14383,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A368" s="11">
         <v>56</v>
       </c>
@@ -14408,7 +14409,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A369" s="11">
         <v>57</v>
       </c>
@@ -14434,7 +14435,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A370" s="11">
         <v>58</v>
       </c>
@@ -14460,7 +14461,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A371" s="11">
         <v>59</v>
       </c>
@@ -14486,7 +14487,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A372" s="11">
         <v>60</v>
       </c>
@@ -14512,7 +14513,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A373" s="11">
         <v>61</v>
       </c>
@@ -14538,7 +14539,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A374" s="11">
         <v>62</v>
       </c>
@@ -14564,7 +14565,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A375" s="11">
         <v>63</v>
       </c>
@@ -14590,7 +14591,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A376" s="11">
         <v>64</v>
       </c>
@@ -14616,7 +14617,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A377" s="11">
         <v>65</v>
       </c>
@@ -14642,7 +14643,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A378" s="11">
         <v>66</v>
       </c>
@@ -14668,7 +14669,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A379" s="11">
         <v>67</v>
       </c>
@@ -14694,7 +14695,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A380" s="11">
         <v>68</v>
       </c>
@@ -14720,7 +14721,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A381" s="11">
         <v>69</v>
       </c>
@@ -14746,7 +14747,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A382" s="11">
         <v>70</v>
       </c>
@@ -14772,7 +14773,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A383" s="11">
         <v>71</v>
       </c>
@@ -14798,7 +14799,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A384" s="11">
         <v>72</v>
       </c>
@@ -14824,7 +14825,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A385" s="11">
         <v>73</v>
       </c>
@@ -14850,7 +14851,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A386" s="11">
         <v>74</v>
       </c>
@@ -14876,7 +14877,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A387" s="11">
         <v>75</v>
       </c>
@@ -14902,7 +14903,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A388" s="11">
         <v>76</v>
       </c>
@@ -14928,7 +14929,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A389" s="11">
         <v>77</v>
       </c>
@@ -14954,7 +14955,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A390" s="11">
         <v>78</v>
       </c>
@@ -14980,7 +14981,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A391" s="1">
         <v>79</v>
       </c>
@@ -15004,7 +15005,7 @@
       </c>
       <c r="H391" s="1"/>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A392" s="1">
         <v>80</v>
       </c>
@@ -15028,12 +15029,12 @@
       </c>
       <c r="H392" s="1"/>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B394" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A395" s="4" t="s">
         <v>1071</v>
       </c>
@@ -15059,7 +15060,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A396" s="1">
         <v>1</v>
       </c>
@@ -15085,7 +15086,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A397" s="1">
         <v>2</v>
       </c>
@@ -15111,7 +15112,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A398" s="1">
         <v>3</v>
       </c>
@@ -15137,7 +15138,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A399" s="1">
         <v>4</v>
       </c>
@@ -15163,7 +15164,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>5</v>
       </c>
@@ -15189,7 +15190,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>6</v>
       </c>
@@ -15215,7 +15216,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A402" s="1">
         <v>7</v>
       </c>
@@ -15241,7 +15242,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A403" s="1">
         <v>8</v>
       </c>
@@ -15267,7 +15268,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>9</v>
       </c>
@@ -15293,7 +15294,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>10</v>
       </c>
@@ -15319,7 +15320,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A406" s="1">
         <v>11</v>
       </c>
@@ -15345,7 +15346,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>12</v>
       </c>
@@ -15371,7 +15372,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>13</v>
       </c>
@@ -15397,7 +15398,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>14</v>
       </c>
@@ -15423,7 +15424,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A410" s="1">
         <v>15</v>
       </c>
@@ -15449,7 +15450,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>16</v>
       </c>
@@ -15475,7 +15476,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
         <v>17</v>
       </c>
@@ -15501,7 +15502,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
         <v>18</v>
       </c>
@@ -15527,7 +15528,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A414" s="11">
         <v>19</v>
       </c>
@@ -15553,7 +15554,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A415" s="11">
         <v>20</v>
       </c>
@@ -15579,7 +15580,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A416" s="11">
         <v>21</v>
       </c>
@@ -15605,7 +15606,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A417" s="11">
         <v>22</v>
       </c>
@@ -15631,7 +15632,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A418" s="11">
         <v>23</v>
       </c>
@@ -15657,7 +15658,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A419" s="11">
         <v>24</v>
       </c>
@@ -15683,7 +15684,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A420" s="11">
         <v>25</v>
       </c>
@@ -15709,7 +15710,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A421" s="11">
         <v>26</v>
       </c>
@@ -15735,7 +15736,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A422" s="11">
         <v>27</v>
       </c>
@@ -15761,7 +15762,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A423" s="11">
         <v>28</v>
       </c>
@@ -15787,7 +15788,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A424" s="11">
         <v>29</v>
       </c>
@@ -15813,7 +15814,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A425" s="11">
         <v>30</v>
       </c>
@@ -15839,12 +15840,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B427" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A428" s="4" t="s">
         <v>1071</v>
       </c>
@@ -15870,7 +15871,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>1</v>
       </c>
@@ -15896,7 +15897,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A430" s="1">
         <v>2</v>
       </c>
@@ -15922,7 +15923,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>3</v>
       </c>
@@ -15948,7 +15949,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A432" s="1">
         <v>4</v>
       </c>
@@ -15974,7 +15975,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A433" s="1">
         <v>5</v>
       </c>
@@ -16000,7 +16001,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>6</v>
       </c>
@@ -16026,7 +16027,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>7</v>
       </c>
@@ -16052,7 +16053,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A436" s="1">
         <v>8</v>
       </c>
@@ -16078,7 +16079,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>9</v>
       </c>
@@ -16104,7 +16105,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A438" s="1">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Add is_train.sql and Update META_DATA
</commit_message>
<xml_diff>
--- a/dataset_competition/META_DATA.xlsx
+++ b/dataset_competition/META_DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="465" windowWidth="22380" windowHeight="14760" tabRatio="681" activeTab="3"/>
+    <workbookView xWindow="2715" yWindow="465" windowWidth="22380" windowHeight="14760" tabRatio="681"/>
   </bookViews>
   <sheets>
     <sheet name="테이블" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3475" uniqueCount="1455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="1458">
   <si>
     <t>SPX</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -4569,6 +4569,18 @@
   </si>
   <si>
     <t>aGLRMLMEX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>글로벌지수 변수 합</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이외 변수 합</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>총 변수 합</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -5618,10 +5630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5730,9 +5742,7 @@
       <c r="C6" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="6" t="s">
         <v>1065</v>
       </c>
@@ -5747,9 +5757,7 @@
       <c r="C7" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="6" t="s">
         <v>1065</v>
       </c>
@@ -5764,9 +5772,7 @@
       <c r="C8" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="6" t="s">
         <v>1066</v>
       </c>
@@ -5922,6 +5928,33 @@
       </c>
       <c r="E17" s="9" t="s">
         <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D19" s="1">
+        <f>SUM(D2:D8)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D20" s="1">
+        <f>SUM(D9:D17)</f>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D21" s="1">
+        <f>SUM(D19:D20)</f>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -5938,6 +5971,7 @@
     <hyperlink ref="E17" location="OTHER_IDX" display="OTHER_IDX"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6135,8 +6169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B321" sqref="B321"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>